<commit_message>
new march db upd
</commit_message>
<xml_diff>
--- a/DATA/ifb.xlsx
+++ b/DATA/ifb.xlsx
@@ -5,8 +5,8 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Tabulado" sheetId="1" r:id="R43620ab332204cea"/>
-    <sheet name="MetaInfo" sheetId="2" r:id="Re8755662f28444b2"/>
+    <sheet name="Tabulado" sheetId="1" r:id="Rc2b64bb4b69a4795"/>
+    <sheet name="MetaInfo" sheetId="2" r:id="R10dbece2ca294123"/>
   </sheets>
 </workbook>
 </file>
@@ -46,7 +46,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -57,7 +57,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -68,7 +68,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -79,7 +79,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -90,7 +90,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -101,7 +101,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -112,7 +112,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -123,7 +123,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -134,7 +134,7 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve">P. Cifras preliminares</t>
+          <t xml:space="preserve">R. Cifras revisadas</t>
         </d:r>
       </text>
     </comment>
@@ -156,6 +156,17 @@
             <sz val="11"/>
             <rFont val="Calibri"/>
           </rPr>
+          <t xml:space="preserve">R. Cifras revisadas</t>
+        </d:r>
+      </text>
+    </comment>
+    <comment ref="NM6" authorId="0">
+      <text>
+        <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+          </rPr>
           <t xml:space="preserve">P. Cifras preliminares</t>
         </d:r>
       </text>
@@ -165,12 +176,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Instituto Nacional de Estadística y Geografía (INEGI).</t>
   </si>
   <si>
-    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Formación Bruta de Capital Fijo. Año Base 2013. Serie de enero de 1993 a noviembre de 2021</t>
+    <t>Sistema de Cuentas Nacionales de México. Indicador Mensual de la Formación Bruta de Capital Fijo. Año Base 2013. Serie de enero de 1993 a diciembre de 2021</t>
   </si>
   <si>
     <t>Índice de volumen físico base 2013=100</t>
@@ -355,7 +366,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -375,7 +386,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -395,7 +406,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -415,7 +426,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -435,7 +446,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -455,7 +466,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -475,7 +486,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -495,7 +506,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -515,7 +526,7 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
-      <d:t xml:space="preserve">P</d:t>
+      <d:t xml:space="preserve">R</d:t>
     </d:r>
   </si>
   <si>
@@ -555,14 +566,31 @@
         <d:color rgb="FF000000"/>
         <d:rFont val="Arial"/>
       </d:rPr>
+      <d:t xml:space="preserve">R</d:t>
+    </d:r>
+  </si>
+  <si>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:sz val="10"/>
+        <d:rFont val="Calibri"/>
+      </d:rPr>
+      <d:t> Diciembre</d:t>
+    </d:r>
+    <d:r xmlns:d="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+      <d:rPr>
+        <d:b/>
+        <d:vertAlign val="superscript"/>
+        <d:sz val="11"/>
+        <d:color rgb="FF000000"/>
+        <d:rFont val="Arial"/>
+      </d:rPr>
       <d:t xml:space="preserve">P</d:t>
     </d:r>
   </si>
   <si>
     <t xml:space="preserve">     Total</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t xml:space="preserve">     Construcción</t>
@@ -625,6 +653,9 @@
       </d:rPr>
       <d:t xml:space="preserve">Cifras revisadas</d:t>
     </d:r>
+  </si>
+  <si>
+    <t>Nota: El Indicador Mensual de la Formación Bruta de Capital Fijo se actualiza una vez teniendo la última información estadística de encuestas, registros administrativos y datos primarios de 2021 y se hace con base en los ´´Lineamientos de cambios a la información divulgada en las publicaciones estadísticas y geográficas del INEGI´´ que se complementan con las ´´Normas Especiales para la Divulgación de Datos´´ del FMI. Incorporar la información más reciente permite identificar posibles diferencias en los niveles de los índices y variaciones que fueron publicados oportunamente.</t>
   </si>
   <si>
     <t>Fuente: INEGI. Sistema de Cuentas Nacionales de México. Indicador Mensual de la Formación Bruta de Capital Fijo</t>
@@ -693,19 +724,19 @@
     <t>COBERTURA TEMPORAL</t>
   </si>
   <si>
-    <t>1993-01-2021-11</t>
+    <t>1993-01-2021-12</t>
   </si>
   <si>
     <t>DESCRIPCIÓN PERIODO</t>
   </si>
   <si>
-    <t>Serie de enero de 1993 a noviembre de 2021</t>
+    <t>Serie de enero de 1993 a diciembre de 2021</t>
   </si>
   <si>
     <t>FECHA DE ACTUALIZACIÓN</t>
   </si>
   <si>
-    <t>2022-02-04</t>
+    <t>2022-03-04</t>
   </si>
 </sst>
 </file>
@@ -798,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" xfId="0"/>
     <xf numFmtId="0" fontId="2" xfId="0"/>
@@ -829,12 +860,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="1" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="6" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -846,7 +871,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:NN24"/>
+  <dimension ref="A1:NN25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2815,7 +2840,7 @@
         <v>56</v>
       </c>
       <c r="NM6" s="10" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="NN6" s="10" t="s">
         <v>45</v>
@@ -2823,7 +2848,7 @@
     </row>
     <row r="7">
       <c r="A7" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" s="11">
         <v>59.351249100159</v>
@@ -3918,13 +3943,13 @@
         <v>84.786187127075</v>
       </c>
       <c r="NB7" s="11">
-        <v>90.4885169009836</v>
+        <v>90.5002119835422</v>
       </c>
       <c r="NC7" s="11">
-        <v>90.8223160591197</v>
+        <v>90.8340111416783</v>
       </c>
       <c r="ND7" s="11">
-        <v>93.7635218275728</v>
+        <v>93.7752169101313</v>
       </c>
       <c r="NE7" s="11">
         <v>88.9215130572554</v>
@@ -3933,28 +3958,28 @@
         <v>93.8208557584863</v>
       </c>
       <c r="NG7" s="11">
-        <v>91.5513777774452</v>
+        <v>91.5484540068055</v>
       </c>
       <c r="NH7" s="11">
-        <v>92.2122408149394</v>
+        <v>92.2005457323808</v>
       </c>
       <c r="NI7" s="11">
-        <v>97.0203561634561</v>
+        <v>97.0031289215855</v>
       </c>
       <c r="NJ7" s="11">
-        <v>94.0030074632734</v>
+        <v>94.0030513552716</v>
       </c>
       <c r="NK7" s="11">
-        <v>93.9223961685321</v>
+        <v>93.9257124999928</v>
       </c>
       <c r="NL7" s="11">
-        <v>95.2334549363054</v>
-      </c>
-      <c r="NM7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN7" s="14" t="s">
-        <v>58</v>
+        <v>95.2097725782645</v>
+      </c>
+      <c r="NM7" s="11">
+        <v>97.7808999787037</v>
+      </c>
+      <c r="NN7" s="11">
+        <v>93.2936144936748</v>
       </c>
     </row>
     <row r="8">
@@ -5054,13 +5079,13 @@
         <v>79.4991325986992</v>
       </c>
       <c r="NB8" s="12">
-        <v>86.9209032688321</v>
+        <v>86.9399397913844</v>
       </c>
       <c r="NC8" s="12">
-        <v>88.8049742815979</v>
+        <v>88.8240108041502</v>
       </c>
       <c r="ND8" s="12">
-        <v>80.9865787296859</v>
+        <v>81.0056152522382</v>
       </c>
       <c r="NE8" s="12">
         <v>80.8502055340998</v>
@@ -5069,13 +5094,13 @@
         <v>84.8490764586654</v>
       </c>
       <c r="NG8" s="12">
-        <v>79.7725301365997</v>
+        <v>79.7677710059616</v>
       </c>
       <c r="NH8" s="12">
-        <v>81.0923735862815</v>
+        <v>81.0733370637292</v>
       </c>
       <c r="NI8" s="12">
-        <v>90.4314312640628</v>
+        <v>90.4028764802343</v>
       </c>
       <c r="NJ8" s="12">
         <v>84.4936834601069</v>
@@ -5086,11 +5111,11 @@
       <c r="NL8" s="12">
         <v>83.3096773075979</v>
       </c>
-      <c r="NM8" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN8" s="15" t="s">
-        <v>58</v>
+      <c r="NM8" s="12">
+        <v>83.6701344390211</v>
+      </c>
+      <c r="NN8" s="12">
+        <v>83.9725244417656</v>
       </c>
     </row>
     <row r="9">
@@ -6222,11 +6247,11 @@
       <c r="NL9" s="11">
         <v>100.17625052363</v>
       </c>
-      <c r="NM9" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN9" s="14" t="s">
-        <v>58</v>
+      <c r="NM9" s="11">
+        <v>102.672613644754</v>
+      </c>
+      <c r="NN9" s="11">
+        <v>102.391305835686</v>
       </c>
     </row>
     <row r="10">
@@ -7326,13 +7351,13 @@
         <v>67.4321256552352</v>
       </c>
       <c r="NB10" s="12">
-        <v>75.5759213599844</v>
+        <v>75.6089162226819</v>
       </c>
       <c r="NC10" s="12">
-        <v>70.6616141993103</v>
+        <v>70.6946090620078</v>
       </c>
       <c r="ND10" s="12">
-        <v>66.8765370755598</v>
+        <v>66.9095319382572</v>
       </c>
       <c r="NE10" s="12">
         <v>66.3307710665326</v>
@@ -7341,13 +7366,13 @@
         <v>66.1672356963311</v>
       </c>
       <c r="NG10" s="12">
-        <v>67.6816124747687</v>
+        <v>67.6733637590943</v>
       </c>
       <c r="NH10" s="12">
-        <v>65.7552289921253</v>
+        <v>65.7222341294279</v>
       </c>
       <c r="NI10" s="12">
-        <v>77.4763069775812</v>
+        <v>77.426814683535</v>
       </c>
       <c r="NJ10" s="12">
         <v>76.9356052472857</v>
@@ -7358,11 +7383,11 @@
       <c r="NL10" s="12">
         <v>70.9424308535965</v>
       </c>
-      <c r="NM10" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN10" s="15" t="s">
-        <v>58</v>
+      <c r="NM10" s="12">
+        <v>69.7367562379908</v>
+      </c>
+      <c r="NN10" s="12">
+        <v>70.4671368349656</v>
       </c>
     </row>
     <row r="11">
@@ -8483,22 +8508,22 @@
         <v>109.926444757163</v>
       </c>
       <c r="NI11" s="11">
-        <v>107.516664889791</v>
+        <v>107.517482682477</v>
       </c>
       <c r="NJ11" s="11">
-        <v>109.15157904969</v>
+        <v>109.15169286265</v>
       </c>
       <c r="NK11" s="11">
-        <v>112.144078663581</v>
+        <v>112.152677987242</v>
       </c>
       <c r="NL11" s="11">
-        <v>114.228306613338</v>
-      </c>
-      <c r="NM11" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN11" s="14" t="s">
-        <v>58</v>
+        <v>114.166897714904</v>
+      </c>
+      <c r="NM11" s="11">
+        <v>120.259673637678</v>
+      </c>
+      <c r="NN11" s="11">
+        <v>108.142325071605</v>
       </c>
     </row>
     <row r="12">
@@ -9630,11 +9655,11 @@
       <c r="NL12" s="12">
         <v>99.0761975356199</v>
       </c>
-      <c r="NM12" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN12" s="15" t="s">
-        <v>58</v>
+      <c r="NM12" s="12">
+        <v>104.437813032906</v>
+      </c>
+      <c r="NN12" s="12">
+        <v>103.74068267103</v>
       </c>
     </row>
     <row r="13">
@@ -10766,11 +10791,11 @@
       <c r="NL13" s="11">
         <v>77.4387694087301</v>
       </c>
-      <c r="NM13" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN13" s="14" t="s">
-        <v>58</v>
+      <c r="NM13" s="11">
+        <v>88.2600259822298</v>
+      </c>
+      <c r="NN13" s="11">
+        <v>100.370364321608</v>
       </c>
     </row>
     <row r="14">
@@ -11902,11 +11927,11 @@
       <c r="NL14" s="12">
         <v>126.530900142876</v>
       </c>
-      <c r="NM14" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN14" s="15" t="s">
-        <v>58</v>
+      <c r="NM14" s="12">
+        <v>124.965036957817</v>
+      </c>
+      <c r="NN14" s="12">
+        <v>108.017119197244</v>
       </c>
     </row>
     <row r="15">
@@ -13027,22 +13052,22 @@
         <v>113.649535976562</v>
       </c>
       <c r="NI15" s="11">
-        <v>111.518513235083</v>
+        <v>111.51987191663</v>
       </c>
       <c r="NJ15" s="11">
-        <v>108.609211679138</v>
+        <v>108.609400768097</v>
       </c>
       <c r="NK15" s="11">
-        <v>113.111546748763</v>
+        <v>113.12583367328</v>
       </c>
       <c r="NL15" s="11">
-        <v>124.249925981332</v>
-      </c>
-      <c r="NM15" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN15" s="14" t="s">
-        <v>58</v>
+        <v>124.147901179016</v>
+      </c>
+      <c r="NM15" s="11">
+        <v>130.724267303233</v>
+      </c>
+      <c r="NN15" s="11">
+        <v>111.053575545472</v>
       </c>
     </row>
     <row r="16">
@@ -14163,22 +14188,22 @@
         <v>87.7230286806358</v>
       </c>
       <c r="NI16" s="12">
-        <v>92.20618371475</v>
+        <v>92.130290841107</v>
       </c>
       <c r="NJ16" s="12">
         <v>87.4908710966149</v>
       </c>
       <c r="NK16" s="12">
-        <v>83.1138957514747</v>
+        <v>83.1390620436592</v>
       </c>
       <c r="NL16" s="12">
-        <v>107.673454681842</v>
-      </c>
-      <c r="NM16" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN16" s="15" t="s">
-        <v>58</v>
+        <v>107.697857919682</v>
+      </c>
+      <c r="NM16" s="12">
+        <v>96.6822956165434</v>
+      </c>
+      <c r="NN16" s="12">
+        <v>89.647292812724</v>
       </c>
     </row>
     <row r="17">
@@ -15299,22 +15324,22 @@
         <v>117.939822657504</v>
       </c>
       <c r="NI17" s="11">
-        <v>114.714293876622</v>
+        <v>114.728436050929</v>
       </c>
       <c r="NJ17" s="11">
-        <v>112.103848819831</v>
+        <v>112.104069199</v>
       </c>
       <c r="NK17" s="11">
-        <v>118.075521304389</v>
+        <v>118.088007924465</v>
       </c>
       <c r="NL17" s="11">
-        <v>126.99298015448</v>
-      </c>
-      <c r="NM17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="NN17" s="14" t="s">
-        <v>58</v>
+        <v>126.870034194886</v>
+      </c>
+      <c r="NM17" s="11">
+        <v>136.357491094366</v>
+      </c>
+      <c r="NN17" s="11">
+        <v>114.595861000606</v>
       </c>
     </row>
     <row r="21">
@@ -15333,7 +15358,12 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3"/>
+      <c r="A24" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3"/>
     </row>
   </sheetData>
   <mergeCells>
@@ -15369,7 +15399,7 @@
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <headerFooter/>
-  <legacyDrawing r:id="Re0aa76917c3f4702"/>
+  <legacyDrawing r:id="R819da3f4254f42dc"/>
 </worksheet>
 </file>
 
@@ -15385,107 +15415,107 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="16" t="s">
-        <v>70</v>
+      <c r="B2" s="14" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="16" t="s">
-        <v>72</v>
+      <c r="B3" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="16" t="s">
-        <v>74</v>
+      <c r="B4" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="16" t="s">
-        <v>76</v>
+      <c r="B5" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="16" t="s">
-        <v>78</v>
+      <c r="B6" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="16" t="s">
-        <v>80</v>
+      <c r="B7" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="16" t="s">
-        <v>82</v>
+      <c r="B8" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="16" t="s">
-        <v>84</v>
+      <c r="B9" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="16" t="s">
-        <v>86</v>
+      <c r="B10" s="14" t="s">
+        <v>87</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="16" t="s">
-        <v>88</v>
+      <c r="B11" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="16" t="s">
-        <v>90</v>
+      <c r="B12" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="16" t="s">
-        <v>92</v>
+      <c r="B13" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="16" t="s">
-        <v>94</v>
+      <c r="B14" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>